<commit_message>
refactor: create snapshot handler (part II)
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance\tools\snapshot-creator-v2\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D0D313-A305-4EB2-8B1E-6676F9B7FEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD48B25-F59C-4704-B504-00175CAB54C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="2730" windowWidth="35550" windowHeight="11010" tabRatio="318" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="1425" yWindow="585" windowWidth="23130" windowHeight="14835" tabRatio="318" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,13 @@
   </sheets>
   <definedNames>
     <definedName name="kc_">heavy!#REF!</definedName>
-    <definedName name="ma1_">heavy!$H$3</definedName>
-    <definedName name="ma2_">heavy!$H$4</definedName>
-    <definedName name="ma3_">heavy!$H$5</definedName>
-    <definedName name="mc1_">heavy!$H$6</definedName>
-    <definedName name="mc2_">heavy!$H$7</definedName>
-    <definedName name="mc3_">heavy!$H$8</definedName>
-    <definedName name="me_">heavy!$H$2</definedName>
+    <definedName name="ma1_">heavy!$I$3</definedName>
+    <definedName name="ma2_">heavy!$I$4</definedName>
+    <definedName name="ma3_">heavy!$I$5</definedName>
+    <definedName name="mc1_">heavy!$I$6</definedName>
+    <definedName name="mc2_">heavy!$I$7</definedName>
+    <definedName name="mc3_">heavy!$I$8</definedName>
+    <definedName name="me_">heavy!$I$2</definedName>
     <definedName name="na_">heavy!#REF!</definedName>
     <definedName name="na1_">heavy!$D$3</definedName>
     <definedName name="na2_">heavy!$D$4</definedName>
@@ -34,7 +34,7 @@
     <definedName name="nc1_">heavy!$D$6</definedName>
     <definedName name="nc2_">heavy!$D$7</definedName>
     <definedName name="nc3_">heavy!$D$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">heavy!$A$1:$P$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">heavy!$A$1:$Q$10</definedName>
     <definedName name="ra1_">heavy!$F$3</definedName>
     <definedName name="ra2_">heavy!$F$4</definedName>
     <definedName name="ra3_">heavy!$F$5</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>CorrectionSentMessages</t>
+  </si>
+  <si>
+    <t>Relationship Hint - Connector Identity Amount</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -354,6 +357,11 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -837,11 +845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B50230-BD5E-4064-AF79-EFC0F2FDB528}">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,27 +860,28 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -891,62 +900,65 @@
       <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -965,60 +977,61 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="11">
         <v>0</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="11"/>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="11">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11">
         <v>50</v>
       </c>
-      <c r="O2" s="11">
-        <v>1</v>
-      </c>
-      <c r="P2" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="9">
+      <c r="P2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
         <f>na1_*ma1_+na2_*ma2_+na3_*ma3_</f>
         <v>775000</v>
       </c>
-      <c r="R2" s="9">
-        <f>na1_*I3+na2_*I4+na3_*I5</f>
+      <c r="S2" s="9">
+        <f>na1_*J3+na2_*J4+na3_*J5</f>
         <v>779500</v>
       </c>
-      <c r="S2" s="10">
-        <f>U2-R2</f>
+      <c r="T2" s="10">
+        <f>V2-S2</f>
         <v>500</v>
       </c>
-      <c r="T2" s="9">
+      <c r="U2" s="9">
         <f>na1_*ra1_+na2_*ra2_+na3_*ra3_</f>
         <v>20500</v>
       </c>
-      <c r="U2" s="9">
+      <c r="V2" s="9">
         <f>nc1_*mc1_+nc2_*mc2_+nc3_*mc3_</f>
         <v>780000</v>
       </c>
-      <c r="V2" s="9">
-        <f>nc1_*I6+nc2_*I7+nc3_*I8</f>
+      <c r="W2" s="9">
+        <f>nc1_*J6+nc2_*J7+nc3_*J8</f>
         <v>774990</v>
       </c>
-      <c r="W2" s="10">
-        <f>Q2-V2</f>
+      <c r="X2" s="10">
+        <f>R2-W2</f>
         <v>10</v>
       </c>
-      <c r="X2" s="9">
+      <c r="Y2" s="9">
         <f>nc1_*rc_1+nc2_*rc_2+nc3_*rc_3</f>
         <v>20530</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1037,38 +1050,42 @@
       <c r="F3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="22">
-        <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na1_)*M3)+L3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="str">
-        <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
+      <c r="G3" s="25" t="str">
+        <f>IF(AND(D6&lt;F3,D7&lt;F3,D8&lt;F3), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="22">
+        <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na1_)*N3)+M3</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="16" t="str">
+        <f t="shared" ref="K3:K8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v>Messages must be 0 on 0 Relationships</v>
       </c>
-      <c r="K3" s="23">
-        <v>0</v>
-      </c>
       <c r="L3" s="23">
         <v>0</v>
       </c>
-      <c r="M3" s="20">
-        <v>0</v>
-      </c>
-      <c r="N3" s="11">
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="20">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11">
         <v>50</v>
       </c>
-      <c r="O3" s="11">
-        <v>1</v>
-      </c>
-      <c r="P3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P3" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1087,39 +1104,43 @@
       <c r="F4" s="11">
         <v>2</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11">
-        <f>50+K4</f>
+      <c r="G4" s="25" t="str">
+        <f>IF(AND(D6&lt;F4,D7&lt;F4,D8&lt;F4), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
+        <f>50+L4</f>
         <v>50</v>
       </c>
-      <c r="I4" s="22">
-        <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na2_)*M4)+L4</f>
+      <c r="J4" s="22">
+        <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na2_)*N4)+M4</f>
         <v>130</v>
       </c>
-      <c r="J4" s="16" t="str">
+      <c r="K4" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="23">
-        <v>0</v>
-      </c>
       <c r="L4" s="23">
         <v>0</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="23">
+        <v>0</v>
+      </c>
+      <c r="N4" s="20">
         <v>0.25</v>
       </c>
-      <c r="N4" s="11">
+      <c r="O4" s="11">
         <v>500</v>
       </c>
-      <c r="O4" s="11">
+      <c r="P4" s="11">
         <v>2</v>
       </c>
-      <c r="P4" s="12">
+      <c r="Q4" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1138,39 +1159,43 @@
       <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
-        <f>200+K5</f>
+      <c r="G5" s="25" t="str">
+        <f>IF(AND(D6&lt;F5,D7&lt;F5,D8&lt;F5), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <f>200+L5</f>
         <v>200</v>
       </c>
-      <c r="I5" s="22">
-        <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na3_)*M5)+L5</f>
+      <c r="J5" s="22">
+        <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na3_)*N5)+M5</f>
         <v>167</v>
       </c>
-      <c r="J5" s="16" t="str">
+      <c r="K5" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="23">
-        <v>0</v>
-      </c>
       <c r="L5" s="23">
         <v>0</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="23">
+        <v>0</v>
+      </c>
+      <c r="N5" s="20">
         <v>0.75</v>
       </c>
-      <c r="N5" s="11">
+      <c r="O5" s="11">
         <v>1500</v>
       </c>
-      <c r="O5" s="11">
+      <c r="P5" s="11">
         <v>3</v>
       </c>
-      <c r="P5" s="12">
+      <c r="Q5" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1187,43 +1212,44 @@
         <v>0</v>
       </c>
       <c r="F6" s="22">
-        <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*G6)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="18">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22">
-        <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc1_)*M6)+L6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="16" t="str">
+        <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*H6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="18">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="22">
+        <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc1_)*N6)+M6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Messages must be 0 on 0 Relationships</v>
       </c>
-      <c r="K6" s="23">
-        <v>0</v>
-      </c>
       <c r="L6" s="23">
         <v>0</v>
       </c>
-      <c r="M6" s="20">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11">
+      <c r="M6" s="23">
+        <v>0</v>
+      </c>
+      <c r="N6" s="20">
         <v>0</v>
       </c>
       <c r="O6" s="11">
-        <v>1</v>
-      </c>
-      <c r="P6" s="12">
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1240,44 +1266,45 @@
         <v>8000</v>
       </c>
       <c r="F7" s="21">
-        <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*G7)</f>
+        <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*H7)</f>
         <v>257</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="26"/>
+      <c r="H7" s="19">
         <v>0.25</v>
       </c>
-      <c r="H7" s="11">
-        <f>12000+K7</f>
+      <c r="I7" s="11">
+        <f>12000+L7</f>
         <v>12000</v>
       </c>
-      <c r="I7" s="22">
-        <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc2_)*M7)+L7</f>
+      <c r="J7" s="22">
+        <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc2_)*N7)+M7</f>
         <v>9687</v>
       </c>
-      <c r="J7" s="16" t="str">
+      <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="23">
-        <v>0</v>
-      </c>
       <c r="L7" s="23">
         <v>0</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
         <v>0.25</v>
       </c>
-      <c r="N7" s="11">
-        <v>0</v>
-      </c>
       <c r="O7" s="11">
-        <v>1</v>
-      </c>
-      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1294,44 +1321,45 @@
         <v>12000</v>
       </c>
       <c r="F8" s="21">
-        <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc3_)*G8)</f>
+        <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc3_)*H8)</f>
         <v>513</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="26"/>
+      <c r="H8" s="19">
         <v>0.75</v>
       </c>
-      <c r="H8" s="11">
-        <f>18000+K8</f>
+      <c r="I8" s="11">
+        <f>18000+L8</f>
         <v>18000</v>
       </c>
-      <c r="I8" s="22">
-        <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc3_)*M8)+L8</f>
+      <c r="J8" s="22">
+        <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc3_)*N8)+M8</f>
         <v>19375</v>
       </c>
-      <c r="J8" s="16" t="str">
+      <c r="K8" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="23">
-        <v>0</v>
-      </c>
       <c r="L8" s="23">
         <v>0</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="23">
+        <v>0</v>
+      </c>
+      <c r="N8" s="20">
         <v>0.75</v>
       </c>
-      <c r="N8" s="11">
-        <v>0</v>
-      </c>
       <c r="O8" s="11">
-        <v>1</v>
-      </c>
-      <c r="P8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="12">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1345,18 +1373,23 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="L10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1367,12 +1400,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E26EECF-D978-410A-A017-B2DC302577D6}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,27 +1416,28 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -1422,62 +1456,65 @@
       <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1496,60 +1533,61 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="11">
         <v>0</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="11"/>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="11">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11">
         <v>50</v>
       </c>
-      <c r="O2" s="11">
-        <v>1</v>
-      </c>
-      <c r="P2" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="9">
-        <f>D3*H3+D4*H4+D5*H5</f>
+      <c r="P2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <f>D3*I3+D4*I4+D5*I5</f>
         <v>16500</v>
       </c>
-      <c r="R2" s="13">
-        <f>D3*I3+D4*I4+D5*I5</f>
+      <c r="S2" s="13">
+        <f>D3*J3+D4*J4+D5*J5</f>
         <v>16800</v>
       </c>
-      <c r="S2" s="14">
-        <f>U2-R2</f>
+      <c r="T2" s="14">
+        <f>V2-S2</f>
         <v>-300</v>
       </c>
-      <c r="T2" s="9">
+      <c r="U2" s="9">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>1800</v>
       </c>
-      <c r="U2" s="9">
-        <f>D6*H6+D7*H7+D8*H8</f>
+      <c r="V2" s="9">
+        <f>D6*I6+D7*I7+D8*I8</f>
         <v>16500</v>
       </c>
-      <c r="V2" s="13">
-        <f>D6*I6+D7*I7+D8*I8</f>
+      <c r="W2" s="13">
+        <f>D6*J6+D7*J7+D8*J8</f>
         <v>16499</v>
       </c>
-      <c r="W2" s="10">
-        <f>Q2-V2</f>
-        <v>1</v>
-      </c>
-      <c r="X2" s="9">
+      <c r="X2" s="10">
+        <f>R2-W2</f>
+        <v>1</v>
+      </c>
+      <c r="Y2" s="9">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>1803</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1568,39 +1606,43 @@
       <c r="F3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11">
-        <f>0+K3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="22">
-        <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="str">
-        <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
+      <c r="G3" s="25" t="str">
+        <f>IF(AND(D6&lt;F3,D7&lt;F3,D8&lt;F3), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11">
+        <f>0+L3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="22">
+        <f>_xlfn.FLOOR.MATH((D6*I6+D7*I7+D8*I8)/(D3)*N3)+M3</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="16" t="str">
+        <f t="shared" ref="K3:K8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v>Messages must be 0 on 0 Relationships</v>
       </c>
-      <c r="K3" s="23">
-        <v>0</v>
-      </c>
       <c r="L3" s="23">
         <v>0</v>
       </c>
-      <c r="M3" s="20">
-        <v>0</v>
-      </c>
-      <c r="N3" s="11">
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="20">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11">
         <v>5</v>
       </c>
-      <c r="O3" s="11">
-        <v>1</v>
-      </c>
-      <c r="P3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P3" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1619,39 +1661,43 @@
       <c r="F4" s="11">
         <v>2</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11">
-        <f>10+K4</f>
+      <c r="G4" s="25" t="str">
+        <f>IF(AND(D6&lt;F4,D7&lt;F4,D8&lt;F4), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
+        <f>10+L4</f>
         <v>10</v>
       </c>
-      <c r="I4" s="22">
-        <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
+      <c r="J4" s="22">
+        <f>_xlfn.FLOOR.MATH((D6*I6+D7*I7+D8*I8)/(D4)*N4)+M4</f>
         <v>30</v>
       </c>
-      <c r="J4" s="16" t="str">
+      <c r="K4" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="23">
-        <v>0</v>
-      </c>
       <c r="L4" s="23">
+        <v>0</v>
+      </c>
+      <c r="M4" s="23">
         <v>3</v>
       </c>
-      <c r="M4" s="20">
+      <c r="N4" s="20">
         <v>0.25</v>
       </c>
-      <c r="N4" s="11">
+      <c r="O4" s="11">
         <v>60</v>
       </c>
-      <c r="O4" s="11">
+      <c r="P4" s="11">
         <v>2</v>
       </c>
-      <c r="P4" s="12">
+      <c r="Q4" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1670,39 +1716,43 @@
       <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
-        <f>50+K5</f>
+      <c r="G5" s="25" t="str">
+        <f>IF(AND(D6&lt;F5,D7&lt;F5,D8&lt;F5), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <f>50+L5</f>
         <v>50</v>
       </c>
-      <c r="I5" s="22">
-        <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
+      <c r="J5" s="22">
+        <f>_xlfn.FLOOR.MATH((D6*I6+D7*I7+D8*I8)/(D5)*N5)+M5</f>
         <v>41</v>
       </c>
-      <c r="J5" s="16" t="str">
+      <c r="K5" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="23">
-        <v>0</v>
-      </c>
       <c r="L5" s="23">
         <v>0</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="23">
+        <v>0</v>
+      </c>
+      <c r="N5" s="20">
         <v>0.75</v>
       </c>
-      <c r="N5" s="11">
-        <v>1</v>
-      </c>
       <c r="O5" s="11">
+        <v>1</v>
+      </c>
+      <c r="P5" s="11">
         <v>3</v>
       </c>
-      <c r="P5" s="12">
+      <c r="Q5" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1719,44 +1769,45 @@
         <v>1</v>
       </c>
       <c r="F6" s="21">
-        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
+        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*H6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="26"/>
+      <c r="H6" s="18">
         <v>0.01</v>
       </c>
-      <c r="H6" s="11">
-        <f>0+K6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="22">
-        <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
+      <c r="I6" s="11">
+        <f>0+L6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="22">
+        <f>_xlfn.FLOOR.MATH((D3*I3+D4*I4+D5*I5)/(D6)*N6)+M6</f>
         <v>82</v>
       </c>
-      <c r="J6" s="16" t="str">
+      <c r="K6" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="23">
-        <v>0</v>
-      </c>
       <c r="L6" s="23">
         <v>0</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="23">
+        <v>0</v>
+      </c>
+      <c r="N6" s="20">
         <v>0.01</v>
       </c>
-      <c r="N6" s="11">
-        <v>0</v>
-      </c>
       <c r="O6" s="11">
-        <v>1</v>
-      </c>
-      <c r="P6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1773,44 +1824,45 @@
         <v>20</v>
       </c>
       <c r="F7" s="21">
-        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
+        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*H7)</f>
         <v>29</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="26"/>
+      <c r="H7" s="18">
         <v>0.24</v>
       </c>
-      <c r="H7" s="11">
-        <f>440+K7</f>
+      <c r="I7" s="11">
+        <f>440+L7</f>
         <v>440</v>
       </c>
-      <c r="I7" s="22">
-        <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
+      <c r="J7" s="22">
+        <f>_xlfn.FLOOR.MATH((D3*I3+D4*I4+D5*I5)/(D7)*N7)+M7</f>
         <v>264</v>
       </c>
-      <c r="J7" s="16" t="str">
+      <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="23">
-        <v>0</v>
-      </c>
       <c r="L7" s="23">
         <v>0</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
         <v>0.24</v>
       </c>
-      <c r="N7" s="11">
-        <v>0</v>
-      </c>
       <c r="O7" s="11">
-        <v>1</v>
-      </c>
-      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1827,44 +1879,45 @@
         <v>30</v>
       </c>
       <c r="F8" s="21">
-        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
+        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*H8)</f>
         <v>90</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="26"/>
+      <c r="H8" s="18">
         <v>0.75</v>
       </c>
-      <c r="H8" s="11">
-        <f>660+K8</f>
+      <c r="I8" s="11">
+        <f>660+L8</f>
         <v>660</v>
       </c>
-      <c r="I8" s="22">
-        <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
+      <c r="J8" s="22">
+        <f>_xlfn.FLOOR.MATH((D3*I3+D4*I4+D5*I5)/(D8)*N8)+M8</f>
         <v>825</v>
       </c>
-      <c r="J8" s="16" t="str">
+      <c r="K8" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="23">
-        <v>0</v>
-      </c>
       <c r="L8" s="23">
         <v>0</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="23">
+        <v>0</v>
+      </c>
+      <c r="N8" s="20">
         <v>0.75</v>
       </c>
-      <c r="N8" s="11">
-        <v>0</v>
-      </c>
       <c r="O8" s="11">
-        <v>1</v>
-      </c>
-      <c r="P8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1878,21 +1931,24 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="L10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P10" s="5"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1903,11 +1959,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7916CF-DA95-4AEE-886B-16E22DB90DBC}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,27 +1974,28 @@
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.7109375" customWidth="1"/>
-    <col min="18" max="18" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="42" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="46" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" customWidth="1"/>
+    <col min="8" max="8" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.7109375" customWidth="1"/>
+    <col min="19" max="19" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="42" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="46" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -1957,62 +2014,65 @@
       <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2031,60 +2091,61 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="11">
         <v>0</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="11"/>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="11">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11">
         <v>50</v>
       </c>
-      <c r="O2" s="11">
-        <v>1</v>
-      </c>
-      <c r="P2" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="9">
-        <f>D3*H3+D4*H4+D5*H5</f>
+      <c r="P2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <f>D3*I3+D4*I4+D5*I5</f>
         <v>48</v>
       </c>
-      <c r="R2" s="13">
-        <f>D3*I3+D4*I4+D5*I5</f>
+      <c r="S2" s="13">
+        <f>D3*J3+D4*J4+D5*J5</f>
         <v>45</v>
       </c>
-      <c r="S2" s="14">
-        <f>U2-R2</f>
+      <c r="T2" s="14">
+        <f>V2-S2</f>
         <v>3</v>
       </c>
-      <c r="T2" s="9">
+      <c r="U2" s="9">
         <f>D3*F3+D4*F4+D5*F5</f>
-        <v>22</v>
-      </c>
-      <c r="U2" s="9">
-        <f>D6*H6+D7*H7+D8*H8</f>
+        <v>19</v>
+      </c>
+      <c r="V2" s="9">
+        <f>D6*I6+D7*I7+D8*I8</f>
         <v>48</v>
       </c>
-      <c r="V2" s="13">
-        <f>D6*I6+D7*I7+D8*I8</f>
+      <c r="W2" s="13">
+        <f>D6*J6+D7*J7+D8*J8</f>
         <v>46</v>
       </c>
-      <c r="W2" s="10">
-        <f>Q2-V2</f>
+      <c r="X2" s="10">
+        <f>R2-W2</f>
         <v>2</v>
       </c>
-      <c r="X2" s="9">
+      <c r="Y2" s="9">
         <f>D6*F6+D7*F7+D8*F8</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2103,39 +2164,43 @@
       <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11">
-        <f>0+K3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="22">
-        <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="str">
-        <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
+      <c r="G3" s="25" t="str">
+        <f>IF(AND(D6&lt;F3,D7&lt;F3,D8&lt;F3), "App Relationships must be less than or equal to connector Amount", "")</f>
         <v/>
       </c>
-      <c r="K3" s="23">
-        <v>0</v>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11">
+        <f>0+L3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="22">
+        <f>_xlfn.FLOOR.MATH((D6*I6+D7*I7+D8*I8)/(D3)*N3)+M3</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="16" t="str">
+        <f t="shared" ref="K3:K8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
+        <v/>
       </c>
       <c r="L3" s="23">
         <v>0</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="20">
         <v>0.01</v>
       </c>
-      <c r="N3" s="11">
+      <c r="O3" s="11">
         <v>50</v>
       </c>
-      <c r="O3" s="11">
-        <v>1</v>
-      </c>
-      <c r="P3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P3" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2154,39 +2219,43 @@
       <c r="F4" s="11">
         <v>2</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11">
-        <f>4+K4</f>
+      <c r="G4" s="25" t="str">
+        <f>IF(AND(D6&lt;F4,D7&lt;F4,D8&lt;F4), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
+        <f>4+L4</f>
         <v>4</v>
       </c>
-      <c r="I4" s="22">
-        <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
+      <c r="J4" s="22">
+        <f>_xlfn.FLOOR.MATH((D6*I6+D7*I7+D8*I8)/(D4)*N4)+M4</f>
         <v>4</v>
       </c>
-      <c r="J4" s="16" t="str">
+      <c r="K4" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="23">
-        <v>0</v>
-      </c>
       <c r="L4" s="23">
         <v>0</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="23">
+        <v>0</v>
+      </c>
+      <c r="N4" s="20">
         <v>0.25</v>
       </c>
-      <c r="N4" s="11">
+      <c r="O4" s="11">
         <v>60</v>
       </c>
-      <c r="O4" s="11">
+      <c r="P4" s="11">
         <v>2</v>
       </c>
-      <c r="P4" s="12">
+      <c r="Q4" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2202,42 +2271,46 @@
       <c r="E5" s="11">
         <v>0</v>
       </c>
-      <c r="F5" s="11">
-        <v>5</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
-        <f>12+K5</f>
+      <c r="F5" s="23">
+        <v>4</v>
+      </c>
+      <c r="G5" s="25" t="str">
+        <f>IF(AND(D6&lt;F5,D7&lt;F5,D8&lt;F5), "App Relationships must be less than or equal to connector Amount", "")</f>
+        <v/>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <f>12+L5</f>
         <v>12</v>
       </c>
-      <c r="I5" s="22">
-        <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
+      <c r="J5" s="22">
+        <f>_xlfn.FLOOR.MATH((D6*I6+D7*I7+D8*I8)/(D5)*N5)+M5</f>
         <v>11</v>
       </c>
-      <c r="J5" s="16" t="str">
+      <c r="K5" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="23">
-        <v>0</v>
-      </c>
       <c r="L5" s="23">
         <v>0</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="23">
+        <v>0</v>
+      </c>
+      <c r="N5" s="20">
         <v>0.74</v>
       </c>
-      <c r="N5" s="11">
-        <v>1</v>
-      </c>
       <c r="O5" s="11">
+        <v>1</v>
+      </c>
+      <c r="P5" s="11">
         <v>3</v>
       </c>
-      <c r="P5" s="12">
+      <c r="Q5" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2254,43 +2327,44 @@
         <v>1</v>
       </c>
       <c r="F6" s="21">
-        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="18">
+        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*H6)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="18">
         <v>0.01</v>
       </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22">
-        <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="16" t="str">
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="22">
+        <f>_xlfn.FLOOR.MATH((D3*I3+D4*I4+D5*I5)/(D6)*N6)+M6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="23">
-        <v>0</v>
-      </c>
       <c r="L6" s="23">
         <v>0</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="23">
+        <v>0</v>
+      </c>
+      <c r="N6" s="20">
         <v>0.01</v>
       </c>
-      <c r="N6" s="11">
-        <v>0</v>
-      </c>
       <c r="O6" s="11">
-        <v>1</v>
-      </c>
-      <c r="P6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2307,44 +2381,45 @@
         <v>20</v>
       </c>
       <c r="F7" s="21">
-        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
+        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*H7)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="26"/>
+      <c r="H7" s="18">
         <v>0.24</v>
       </c>
-      <c r="H7" s="11">
-        <f>8+K7</f>
+      <c r="I7" s="11">
+        <f>8+L7</f>
         <v>8</v>
       </c>
-      <c r="I7" s="22">
-        <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
+      <c r="J7" s="22">
+        <f>_xlfn.FLOOR.MATH((D3*I3+D4*I4+D5*I5)/(D7)*N7)+M7</f>
         <v>5</v>
       </c>
-      <c r="J7" s="16" t="str">
+      <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="23">
-        <v>0</v>
-      </c>
       <c r="L7" s="23">
         <v>0</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
         <v>0.24</v>
       </c>
-      <c r="N7" s="11">
-        <v>0</v>
-      </c>
       <c r="O7" s="11">
-        <v>1</v>
-      </c>
-      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2354,51 +2429,52 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="23">
         <v>4</v>
       </c>
       <c r="E8" s="11">
         <v>30</v>
       </c>
       <c r="F8" s="21">
-        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
-        <v>5</v>
-      </c>
-      <c r="G8" s="18">
+        <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*H8)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="18">
         <v>0.75</v>
       </c>
-      <c r="H8" s="11">
-        <f>8+K8</f>
+      <c r="I8" s="11">
+        <f>8+L8</f>
         <v>8</v>
       </c>
-      <c r="I8" s="22">
-        <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
+      <c r="J8" s="22">
+        <f>_xlfn.FLOOR.MATH((D3*I3+D4*I4+D5*I5)/(D8)*N8)+M8</f>
         <v>9</v>
       </c>
-      <c r="J8" s="16" t="str">
+      <c r="K8" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="23">
-        <v>0</v>
-      </c>
       <c r="L8" s="23">
         <v>0</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="23">
+        <v>0</v>
+      </c>
+      <c r="N8" s="20">
         <v>0.75</v>
       </c>
-      <c r="N8" s="11">
-        <v>0</v>
-      </c>
       <c r="O8" s="11">
-        <v>1</v>
-      </c>
-      <c r="P8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2412,21 +2488,24 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="L10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P10" s="5"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test: added light, heavy pool-config and linux drop/restore clean-db script a tiny adjsutment was required in performancetest excel. rule: configured relationship-templates >= configured relationships on connector side, otherwise no relationships can be created in db.
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance\tools\snapshot-creator-v2\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C6DA9-D055-45BE-981D-FBD8B8142A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843E4E73-41D0-456C-941A-4B41B107D4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="22695" windowHeight="12690" tabRatio="318" activeTab="2" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="12405" yWindow="0" windowWidth="20175" windowHeight="10770" tabRatio="318" activeTab="1" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -369,6 +369,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -856,7 +859,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1225,10 @@
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*H6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="26" t="str">
+        <f>IF(E6&lt;F6, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H6" s="18">
         <v>0</v>
       </c>
@@ -1276,7 +1282,10 @@
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*H7)</f>
         <v>257</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="26" t="str">
+        <f t="shared" ref="G7:G8" si="1">IF(E7&lt;F7, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H7" s="19">
         <v>0.25</v>
       </c>
@@ -1331,7 +1340,10 @@
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc3_)*H8)</f>
         <v>513</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="H8" s="19">
         <v>0.75</v>
       </c>
@@ -1409,10 +1421,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E26EECF-D978-410A-A017-B2DC302577D6}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1435,7 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.85546875" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" customWidth="1"/>
     <col min="8" max="8" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
@@ -1540,7 +1552,7 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11">
         <v>0</v>
@@ -1773,13 +1785,16 @@
         <v>2</v>
       </c>
       <c r="E6" s="11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F6" s="21">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*H6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="28" t="str">
+        <f>IF(E6&lt;F6, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H6" s="18">
         <v>0.01</v>
       </c>
@@ -1828,13 +1843,16 @@
         <v>15</v>
       </c>
       <c r="E7" s="11">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F7" s="21">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*H7)</f>
         <v>29</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="28" t="str">
+        <f t="shared" ref="G7:G8" si="1">IF(E7&lt;F7, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H7" s="18">
         <v>0.24</v>
       </c>
@@ -1883,13 +1901,16 @@
         <v>15</v>
       </c>
       <c r="E8" s="11">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F8" s="21">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*H8)</f>
         <v>90</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="H8" s="18">
         <v>0.75</v>
       </c>
@@ -1968,9 +1989,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7916CF-DA95-4AEE-886B-16E22DB90DBC}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2358,10 @@
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*H6)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="26" t="str">
+        <f>IF(E6&lt;F6, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H6" s="18">
         <v>0.01</v>
       </c>
@@ -2391,7 +2415,10 @@
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*H7)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="26" t="str">
+        <f t="shared" ref="G7:G8" si="1">IF(E7&lt;F7, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H7" s="18">
         <v>0.24</v>
       </c>
@@ -2446,7 +2473,10 @@
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*H8)</f>
         <v>4</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="H8" s="18">
         <v>0.75</v>
       </c>

</xml_diff>

<commit_message>
test: added light, heavy pool-config and linux drop/restore clean-db script a tiny adjustment was required in PerformanceTest Excel file. rule: configured relationship-templates >= configured relationships on connector side, otherwise no relationships can be created in db.
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance\tools\snapshot-creator-v2\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C6DA9-D055-45BE-981D-FBD8B8142A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843E4E73-41D0-456C-941A-4B41B107D4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="22695" windowHeight="12690" tabRatio="318" activeTab="2" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="12405" yWindow="0" windowWidth="20175" windowHeight="10770" tabRatio="318" activeTab="1" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -369,6 +369,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -856,7 +859,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1225,10 @@
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*H6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="26" t="str">
+        <f>IF(E6&lt;F6, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H6" s="18">
         <v>0</v>
       </c>
@@ -1276,7 +1282,10 @@
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*H7)</f>
         <v>257</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="26" t="str">
+        <f t="shared" ref="G7:G8" si="1">IF(E7&lt;F7, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H7" s="19">
         <v>0.25</v>
       </c>
@@ -1331,7 +1340,10 @@
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc3_)*H8)</f>
         <v>513</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="H8" s="19">
         <v>0.75</v>
       </c>
@@ -1409,10 +1421,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E26EECF-D978-410A-A017-B2DC302577D6}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1435,7 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.85546875" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" customWidth="1"/>
     <col min="8" max="8" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
@@ -1540,7 +1552,7 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11">
         <v>0</v>
@@ -1773,13 +1785,16 @@
         <v>2</v>
       </c>
       <c r="E6" s="11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F6" s="21">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*H6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="28" t="str">
+        <f>IF(E6&lt;F6, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H6" s="18">
         <v>0.01</v>
       </c>
@@ -1828,13 +1843,16 @@
         <v>15</v>
       </c>
       <c r="E7" s="11">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F7" s="21">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*H7)</f>
         <v>29</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="28" t="str">
+        <f t="shared" ref="G7:G8" si="1">IF(E7&lt;F7, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H7" s="18">
         <v>0.24</v>
       </c>
@@ -1883,13 +1901,16 @@
         <v>15</v>
       </c>
       <c r="E8" s="11">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F8" s="21">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*H8)</f>
         <v>90</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="H8" s="18">
         <v>0.75</v>
       </c>
@@ -1968,9 +1989,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7916CF-DA95-4AEE-886B-16E22DB90DBC}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2358,10 @@
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*H6)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="26" t="str">
+        <f>IF(E6&lt;F6, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H6" s="18">
         <v>0.01</v>
       </c>
@@ -2391,7 +2415,10 @@
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*H7)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="26" t="str">
+        <f t="shared" ref="G7:G8" si="1">IF(E7&lt;F7, "Need at least as much Relationship-Templates as Relationships", "")</f>
+        <v/>
+      </c>
       <c r="H7" s="18">
         <v>0.24</v>
       </c>
@@ -2446,7 +2473,10 @@
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*H8)</f>
         <v>4</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="H8" s="18">
         <v>0.75</v>
       </c>

</xml_diff>